<commit_message>
Principais arquivos Excel, compilador e exemplos
</commit_message>
<xml_diff>
--- a/instructionSet.xlsx
+++ b/instructionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Augusto Manzano\Downloads\excelCPU-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECECE22-7376-4E74-AE11-6799221D7641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C42B0B-79CE-434C-832C-CACCB50DBC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>32b/16b</t>
   </si>
   <si>
-    <t>OPERATION</t>
-  </si>
-  <si>
     <t>ALU OP</t>
   </si>
   <si>
@@ -342,24 +339,12 @@
     <t>NOTAS TÉCNICAS</t>
   </si>
   <si>
-    <t>PC CONFIGURADO PARA O VALOR IMEDIATO ATRAVÉS DO OPERANDO 2 SELECIONADO PELO MUX</t>
-  </si>
-  <si>
-    <t>SALTA SE FLAG ZERO ESTIVER VERDADEIRO</t>
-  </si>
-  <si>
     <t>DEFINE REGISTRO PARA VALOR DE MEMÓRIA NO ENDEREÇO IMEDIATO</t>
   </si>
   <si>
-    <t>DEFINE REGISTRO PARA O VALOR IMEDIATO</t>
-  </si>
-  <si>
     <t>DEFINE VALOR DE MEMÓRIA NO ENDEREÇO IMEDIATO PARA O VALOR DO REGISTRO</t>
   </si>
   <si>
-    <t>DEFINE VALOR DE MEMÓRIA NO ENDEREÇO DE REGB PARA O VALOR DE REGA</t>
-  </si>
-  <si>
     <t>TRANSFERA VALOR DE REGA PARA REGB</t>
   </si>
   <si>
@@ -393,21 +378,9 @@
     <t>MULTIPLIED REGA AND REGB, ARMAZENA RESULTADO DE 16 BITS BAIXO EM REGA, ARMAZENA RESULTADO DE 16 BITS ALTO EM REGB</t>
   </si>
   <si>
-    <t>ROTAÇÃO À ESQUERDA DOS BITS DE REGA REALIZADA 4 VEZES, COM TRANSPORTE (CARRY) DE 4 BITS IMD</t>
-  </si>
-  <si>
-    <t>ROTAÇÃO À DIREITA DOS BITS DE REGA REALIZADA 4 VEZES, COM TRANSPORTE (CARRY) DE 4 BITS IMD</t>
-  </si>
-  <si>
     <t>SUBTRAI REGA E REGB, O RESULTADOS NÃO É ARMAZENADO, APENAS FLAGS SÃO AFETADAS</t>
   </si>
   <si>
-    <t>SALTA SE FLAG DE TRANSPORTE (CARRY) FOR FALSA</t>
-  </si>
-  <si>
-    <t>SALTA SE FLAG DE TRANSPORTE (CARRY) OU FLAG ZERO FOREM VERDADEIRAS</t>
-  </si>
-  <si>
     <t>FLAG DE TRANSPORTE (CARRY) DEFINIDA COMO 0</t>
   </si>
   <si>
@@ -418,6 +391,33 @@
   </si>
   <si>
     <t>DEFINE REGA PARA VALOR DE MEMÓRIA NO ENDEREÇO EM REGB</t>
+  </si>
+  <si>
+    <t>OPERAÇÃO</t>
+  </si>
+  <si>
+    <t>PC CONFIGURADO PARA VALOR IMEDIATO POR MEIO DO OPERANDO 2 SELECIONADO PELO MUX</t>
+  </si>
+  <si>
+    <t>SALTA SE FLAG ZERO ESTIVER VERDADEIRA</t>
+  </si>
+  <si>
+    <t>SALTA SE FLAG DE TRANSPORTE (CARRY) ESTIVER FALSA</t>
+  </si>
+  <si>
+    <t>SALTA SE FLAG DE TRANSPORTE (CARRY) OU FLAG ZERO ESTIVEREM VERDADEIRAS</t>
+  </si>
+  <si>
+    <t>DEFINE REGISTRO PARA VALOR IMEDIATO</t>
+  </si>
+  <si>
+    <t>DEFINE VALOR DE MEMÓRIA NO ENDEREÇO DE REGB PARA VALOR DE REGA</t>
+  </si>
+  <si>
+    <t>ROTAÇÃO À ESQUERDA DOS BITS DE REGA REALIZADA 4 VEZES, COM TRANSPORTE (CARRY) DE 4 BITS EM IMD</t>
+  </si>
+  <si>
+    <t>ROTAÇÃO À DIREITA DOS BITS DE REGA REALIZADA 4 VEZES, COM TRANSPORTE (CARRY) DE 4 BITS EM IMD</t>
   </si>
 </sst>
 </file>
@@ -972,50 +972,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1327,10 +1327,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="37"/>
+      <c r="A2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="36"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1346,56 +1346,56 @@
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="Q2" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="H3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
       <c r="K3" s="10">
         <v>15</v>
       </c>
@@ -1415,30 +1415,30 @@
         <v>0</v>
       </c>
       <c r="Q3" s="28" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="17"/>
       <c r="F4" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+        <v>13</v>
+      </c>
+      <c r="G4" s="40"/>
+      <c r="H4" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="10">
         <v>15</v>
       </c>
@@ -1458,30 +1458,30 @@
         <v>0</v>
       </c>
       <c r="Q4" s="28" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="17"/>
       <c r="F5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
+        <v>13</v>
+      </c>
+      <c r="G5" s="40"/>
+      <c r="H5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
       <c r="K5" s="10">
         <v>15</v>
       </c>
@@ -1506,25 +1506,25 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="14">
         <v>3</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="17"/>
       <c r="F6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+        <v>13</v>
+      </c>
+      <c r="G6" s="40"/>
+      <c r="H6" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
       <c r="K6" s="10">
         <v>15</v>
       </c>
@@ -1549,27 +1549,27 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="14">
         <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="40"/>
+      <c r="H7" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
       <c r="K7" s="10">
         <v>15</v>
       </c>
@@ -1589,32 +1589,32 @@
         <v>1</v>
       </c>
       <c r="Q7" s="28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="14">
         <v>5</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
+        <v>13</v>
+      </c>
+      <c r="G8" s="40"/>
+      <c r="H8" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
       <c r="K8" s="10">
         <v>15</v>
       </c>
@@ -1634,32 +1634,32 @@
         <v>1</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="19">
         <v>6</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+        <v>28</v>
+      </c>
+      <c r="G9" s="40"/>
+      <c r="H9" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
       <c r="K9" s="10">
         <v>12</v>
       </c>
@@ -1679,34 +1679,34 @@
         <v>0</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="22">
         <v>7</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="24"/>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="H10" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
       <c r="K10" s="10">
         <v>12</v>
       </c>
@@ -1726,32 +1726,32 @@
         <v>0</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="14">
         <v>8</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
       <c r="K11" s="10">
         <v>12</v>
       </c>
@@ -1771,35 +1771,35 @@
         <v>0</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="14">
         <v>9</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="31" t="s">
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="L12" s="11">
         <v>1</v>
       </c>
@@ -1816,35 +1816,35 @@
         <v>0</v>
       </c>
       <c r="Q12" s="28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="14">
         <v>10</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="31" t="s">
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="L13" s="11">
         <v>1</v>
       </c>
@@ -1861,35 +1861,35 @@
         <v>0</v>
       </c>
       <c r="Q13" s="28" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="14">
         <v>11</v>
       </c>
       <c r="C14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="31" t="s">
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="L14" s="11">
         <v>1</v>
       </c>
@@ -1906,35 +1906,35 @@
         <v>0</v>
       </c>
       <c r="Q14" s="28" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="14">
         <v>12</v>
       </c>
       <c r="C15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="31" t="s">
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="L15" s="11">
         <v>1</v>
       </c>
@@ -1951,33 +1951,33 @@
         <v>0</v>
       </c>
       <c r="Q15" s="28" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="14">
         <v>13</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="31" t="s">
+      <c r="G16" s="33"/>
+      <c r="H16" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="L16" s="11">
         <v>0</v>
       </c>
@@ -1994,33 +1994,33 @@
         <v>0</v>
       </c>
       <c r="Q16" s="28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="14">
         <v>14</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="31" t="s">
+      <c r="G17" s="33"/>
+      <c r="H17" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="L17" s="11">
         <v>0</v>
       </c>
@@ -2037,35 +2037,35 @@
         <v>0</v>
       </c>
       <c r="Q17" s="28" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="14">
         <v>15</v>
       </c>
       <c r="C18" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="31" t="s">
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="L18" s="11">
         <v>1</v>
       </c>
@@ -2082,35 +2082,35 @@
         <v>0</v>
       </c>
       <c r="Q18" s="28" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="14">
         <v>16</v>
       </c>
       <c r="C19" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="31" t="s">
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="L19" s="11">
         <v>1</v>
       </c>
@@ -2127,35 +2127,35 @@
         <v>0</v>
       </c>
       <c r="Q19" s="28" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="14">
         <v>17</v>
       </c>
       <c r="C20" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="31" t="s">
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="L20" s="11">
         <v>1</v>
       </c>
@@ -2172,33 +2172,33 @@
         <v>0</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="14">
         <v>18</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="31" t="s">
+      <c r="G21" s="33"/>
+      <c r="H21" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="10" t="s">
-        <v>80</v>
-      </c>
       <c r="L21" s="11">
         <v>0</v>
       </c>
@@ -2215,32 +2215,32 @@
         <v>0</v>
       </c>
       <c r="Q21" s="28" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="14">
         <v>19</v>
       </c>
       <c r="C22" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
       <c r="K22" s="10">
         <v>10</v>
       </c>
@@ -2260,32 +2260,32 @@
         <v>0</v>
       </c>
       <c r="Q22" s="28" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="14">
         <v>20</v>
       </c>
       <c r="C23" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
       <c r="K23" s="10">
         <v>11</v>
       </c>
@@ -2305,34 +2305,34 @@
         <v>0</v>
       </c>
       <c r="Q23" s="28" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="14">
         <v>21</v>
       </c>
       <c r="C24" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
       <c r="K24" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L24" s="11">
         <v>1</v>
@@ -2350,28 +2350,28 @@
         <v>0</v>
       </c>
       <c r="Q24" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="14">
         <v>22</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="17"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="31"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="41"/>
+      <c r="J25" s="30"/>
       <c r="K25" s="10">
         <v>13</v>
       </c>
@@ -2391,28 +2391,28 @@
         <v>0</v>
       </c>
       <c r="Q25" s="28" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="14">
         <v>23</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="17"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="I26" s="30"/>
-      <c r="J26" s="31"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="41"/>
+      <c r="J26" s="30"/>
       <c r="K26" s="10">
         <v>14</v>
       </c>
@@ -2432,28 +2432,28 @@
         <v>0</v>
       </c>
       <c r="Q26" s="28" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="14">
         <v>24</v>
       </c>
       <c r="C27" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="42"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
       <c r="K27" s="10">
         <v>15</v>
       </c>
@@ -2473,32 +2473,32 @@
         <v>0</v>
       </c>
       <c r="Q27" s="28" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="19">
         <v>25</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28" s="25"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
       <c r="K28" s="26">
         <v>15</v>
       </c>
@@ -2518,23 +2518,14 @@
         <v>1</v>
       </c>
       <c r="Q28" s="29" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="G10:G28"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="H20:J20"/>
@@ -2549,11 +2540,20 @@
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="G10:G28"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="H26:J26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="H28:J28"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:F26 A27:D27 F27 A28:F28">
     <cfRule type="containsBlanks" dxfId="1" priority="1">

</xml_diff>